<commit_message>
Updated the secondOrderCheck list
</commit_message>
<xml_diff>
--- a/resources/secondOrderCheck.xlsx
+++ b/resources/secondOrderCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\recherche\fuzzyCalculator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C2374-7B8D-48FA-964D-1E4D39900627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23094541-DE4C-4AB8-B55B-2DA00C9F21A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{DB1751ED-BCAF-4A8B-BBB1-B3D9B7C224F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="17">
   <si>
     <t>(</t>
   </si>
@@ -77,20 +77,23 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>Possible for some specific tokens of this kind</t>
-  </si>
-  <si>
-    <t>Combination impossible</t>
-  </si>
-  <si>
-    <t>Possible for any tokens of these kind</t>
+    <t>Internal error: tokenise is not supposed to output that</t>
+  </si>
+  <si>
+    <t>Combination is possible for some specific tokens of this kind</t>
+  </si>
+  <si>
+    <t>Combination is possible for any tokens of this kind</t>
+  </si>
+  <si>
+    <t>Combination is impossible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -121,6 +124,18 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -284,18 +299,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,38 +308,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,14 +690,14 @@
   <dimension ref="A5:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="12" width="7.1328125" customWidth="1"/>
     <col min="15" max="15" width="7.1328125" customWidth="1"/>
-    <col min="16" max="16" width="50.796875" customWidth="1"/>
+    <col min="16" max="16" width="63.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -698,17 +713,17 @@
     </row>
     <row r="6" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="1"/>
@@ -743,342 +758,348 @@
     </row>
     <row r="8" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="str">
+      <c r="C8" s="10" t="str">
         <f>D7</f>
         <v>const</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="27" t="s">
+      <c r="D8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
-      <c r="B9" s="17"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="4" t="str">
         <f>E7</f>
         <v>func</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="19" t="s">
+      <c r="D9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="27" t="s">
+      <c r="O9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="17"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="4" t="str">
         <f>F7</f>
         <v>infix</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="18" t="s">
+      <c r="D10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="27" t="s">
-        <v>13</v>
+      <c r="O10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="17"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="4" t="str">
         <f>G7</f>
         <v>var</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>14</v>
+      <c r="D11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="4" t="str">
         <f>H7</f>
         <v>(</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>3</v>
+      <c r="D12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="17"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="4" t="str">
         <f>I7</f>
         <v>)</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="24" t="s">
+      <c r="D13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="17"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="4" t="str">
         <f>J7</f>
         <v>,</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="24" t="s">
+      <c r="D14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="4" t="str">
         <f>K7</f>
         <v>num</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="24" t="s">
+      <c r="D15" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="6" t="str">
         <f>L7</f>
         <v>" "</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="26" t="s">
+      <c r="D16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="19" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>